<commit_message>
Update box plot scripts
</commit_message>
<xml_diff>
--- a/data/OleA_taxonomic_classification.xlsx
+++ b/data/OleA_taxonomic_classification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robi0916/Documents/University_of_Minnesota/Wackett_Lab/github/synbio-data-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6A3EAEA-B1E7-084B-B031-7B4027BA7143}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3504DD5D-5F88-544B-9FCF-D15635A22A9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="460" windowWidth="24340" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="460" windowWidth="24340" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OleA_taxonomic_classification" sheetId="1" r:id="rId1"/>
@@ -1527,7 +1527,7 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1954,7 +1954,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>112</v>

</xml_diff>